<commit_message>
updates to bugs in Microbit testing
</commit_message>
<xml_diff>
--- a/SN4 comms values.xlsx
+++ b/SN4 comms values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\SN4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDF62DB-9E33-40AB-81A6-15C2AE6EFDA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3429D04-3C0C-471C-890E-2F2C647B58EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MQTT topics" sheetId="1" state="hidden" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="414">
   <si>
     <t>Action</t>
   </si>
@@ -856,12 +856,6 @@
     <t>ADC2</t>
   </si>
   <si>
-    <t>0-4095</t>
-  </si>
-  <si>
-    <t>12-bit value based on voltage, received on change</t>
-  </si>
-  <si>
     <t>Rotary Encoders</t>
   </si>
   <si>
@@ -1275,6 +1269,21 @@
   <si>
     <t>https://funprojects.blog/2019/05/21/control-microbits-from-your-pc/</t>
   </si>
+  <si>
+    <t>0-100</t>
+  </si>
+  <si>
+    <t>12-bit value  mapped to 0-100 to reduce noisy reading based on voltage, received on change</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>turn on/off the ADC sampling due to noise</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
 </sst>
 </file>
 
@@ -1567,7 +1576,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30038,10 +30047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30053,7 +30062,7 @@
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="46" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" s="46" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A1" s="46" t="s">
         <v>258</v>
       </c>
@@ -30070,381 +30079,418 @@
         <v>267</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>366</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="33" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="33" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="33" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="33" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C9" s="49"/>
       <c r="D9" s="33" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="33" t="s">
         <v>105</v>
       </c>
       <c r="B11" s="43" t="s">
+        <v>342</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>343</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>345</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>346</v>
-      </c>
       <c r="E11" s="33" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="33" t="s">
         <v>105</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E12" s="33" t="s">
         <v>348</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>350</v>
-      </c>
       <c r="F12" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="33" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="43" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="51" t="s">
         <v>351</v>
       </c>
-      <c r="C13" s="51" t="s">
-        <v>353</v>
-      </c>
       <c r="D13" s="52" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="33" t="s">
         <v>166</v>
       </c>
       <c r="B14" s="43" t="s">
+        <v>353</v>
+      </c>
+      <c r="C14" s="51" t="s">
         <v>355</v>
       </c>
-      <c r="C14" s="51" t="s">
-        <v>357</v>
-      </c>
       <c r="D14" s="52" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="33" t="s">
         <v>166</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C15" s="51" t="s">
+        <v>355</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="D15" s="52" t="s">
-        <v>360</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>359</v>
-      </c>
       <c r="F15" s="43" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="45" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="45" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>361</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>362</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>364</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="F16" s="54" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="B17" s="54" t="s">
         <v>363</v>
       </c>
-      <c r="C16" s="54" t="s">
-        <v>364</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>366</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="F16" s="54" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="45" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="45" t="s">
-        <v>273</v>
-      </c>
-      <c r="B17" s="54" t="s">
+      <c r="C17" s="54" t="s">
+        <v>362</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="C17" s="54" t="s">
-        <v>364</v>
-      </c>
-      <c r="D17" s="45" t="s">
+      <c r="E17" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="F17" s="54" t="s">
         <v>367</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>276</v>
-      </c>
-      <c r="F17" s="54" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>374</v>
+      </c>
+      <c r="C18" s="51" t="s">
         <v>375</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="D18" s="52" t="s">
         <v>376</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="E18" s="33" t="s">
         <v>377</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>378</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>379</v>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>411</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>362</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>412</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>413</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>362</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>412</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -30458,8 +30504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1F20C5-E431-4F51-B98A-61CA1E4D1DB8}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30467,8 +30513,8 @@
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1875" style="43" customWidth="1"/>
     <col min="3" max="3" width="26.80859375" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.046875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.76171875" style="43"/>
   </cols>
@@ -30493,7 +30539,7 @@
         <v>267</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -30501,7 +30547,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C2" s="47" t="s">
         <v>261</v>
@@ -30511,10 +30557,10 @@
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -30522,20 +30568,20 @@
         <v>8</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E3" s="33"/>
       <c r="F3" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G3" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -30543,20 +30589,20 @@
         <v>8</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C4" s="51" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>300</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>302</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -30564,7 +30610,7 @@
         <v>87</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>264</v>
@@ -30574,10 +30620,10 @@
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="33" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -30585,7 +30631,7 @@
         <v>87</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C6" s="49" t="s">
         <v>264</v>
@@ -30595,10 +30641,10 @@
       </c>
       <c r="E6" s="33"/>
       <c r="F6" s="33" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -30606,20 +30652,20 @@
         <v>268</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>271</v>
+        <v>409</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>272</v>
+        <v>410</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="33" t="s">
         <v>269</v>
       </c>
       <c r="G7" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -30627,62 +30673,62 @@
         <v>268</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>271</v>
+        <v>409</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>272</v>
+        <v>410</v>
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="33" t="s">
         <v>270</v>
       </c>
       <c r="G8" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E9" s="33"/>
       <c r="F9" s="33" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E10" s="33"/>
       <c r="F10" s="33" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G10" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -30690,20 +30736,20 @@
         <v>98</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E11" s="33"/>
       <c r="F11" s="33" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -30711,20 +30757,20 @@
         <v>98</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="33" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -30732,20 +30778,20 @@
         <v>98</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="33" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -30753,20 +30799,20 @@
         <v>98</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E14" s="33"/>
       <c r="F14" s="33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -30774,20 +30820,20 @@
         <v>98</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E15" s="33"/>
       <c r="F15" s="33" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -30795,20 +30841,20 @@
         <v>98</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E16" s="33"/>
       <c r="F16" s="33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -30816,20 +30862,20 @@
         <v>98</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E17" s="33"/>
       <c r="F17" s="33" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -30837,20 +30883,20 @@
         <v>98</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E18" s="33"/>
       <c r="F18" s="33" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G18" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -30858,20 +30904,20 @@
         <v>98</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E19" s="33"/>
       <c r="F19" s="33" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G19" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -30879,20 +30925,20 @@
         <v>98</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E20" s="33"/>
       <c r="F20" s="33" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -30900,20 +30946,20 @@
         <v>98</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E21" s="33"/>
       <c r="F21" s="33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G21" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -30921,20 +30967,20 @@
         <v>98</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E22" s="33"/>
       <c r="F22" s="33" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G22" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -30942,20 +30988,20 @@
         <v>98</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E23" s="33"/>
       <c r="F23" s="33" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G23" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
@@ -30963,20 +31009,20 @@
         <v>98</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E24" s="33"/>
       <c r="F24" s="33" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -30984,20 +31030,20 @@
         <v>98</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E25" s="33"/>
       <c r="F25" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G25" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -31005,54 +31051,54 @@
         <v>98</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E26" s="33"/>
       <c r="F26" s="33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G26" s="43" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B27" s="43" t="s">
+        <v>386</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>387</v>
+      </c>
+      <c r="D27" s="33" t="s">
         <v>388</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="F27" s="33" t="s">
         <v>389</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>390</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C28" s="51" t="s">
+        <v>387</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>391</v>
+      </c>
+      <c r="F28" s="33" t="s">
         <v>389</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>393</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -37022,7 +37068,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="53" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -37073,7 +37119,7 @@
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>62</v>
@@ -37103,7 +37149,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="53" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B8" s="53" t="s">
         <v>88</v>
@@ -37113,12 +37159,12 @@
         <v>90</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="53" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B9" s="53" t="s">
         <v>96</v>
@@ -37128,12 +37174,12 @@
         <v>97</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="53" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B10" s="53" t="s">
         <v>112</v>
@@ -37143,7 +37189,7 @@
         <v>114</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -37158,12 +37204,12 @@
         <v>126</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="53" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B12" s="53" t="s">
         <v>130</v>
@@ -37173,12 +37219,12 @@
         <v>131</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="53" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B13" s="53" t="s">
         <v>133</v>
@@ -37188,12 +37234,12 @@
         <v>134</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="53" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B14" s="53" t="s">
         <v>137</v>
@@ -37203,7 +37249,7 @@
         <v>138</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41210,22 +41256,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -41270,7 +41316,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="53" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -41342,7 +41388,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="53" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>88</v>
@@ -41369,7 +41415,7 @@
         <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41381,7 +41427,7 @@
         <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41393,7 +41439,7 @@
         <v>131</v>
       </c>
       <c r="E12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41405,7 +41451,7 @@
         <v>134</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
updates to get WiFi smoother
</commit_message>
<xml_diff>
--- a/SN4 comms values.xlsx
+++ b/SN4 comms values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\SN4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661DE7E4-DCFB-42FB-8D60-554FBFAB5390}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFFB41D-06AD-4037-B648-286A37ED101F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="444">
   <si>
     <t>Action</t>
   </si>
@@ -1312,9 +1312,6 @@
     <t>https://bit.ly/3mmGDQT</t>
   </si>
   <si>
-    <t>Bitly URL upto 30 characters (</t>
-  </si>
-  <si>
     <t>G2</t>
   </si>
   <si>
@@ -1366,10 +1363,16 @@
     <t>T9</t>
   </si>
   <si>
-    <t>therobotnetwork</t>
+    <t>Reset</t>
   </si>
   <si>
-    <t>isaacasimov</t>
+    <t>START</t>
+  </si>
+  <si>
+    <t>Resets the ESP32</t>
+  </si>
+  <si>
+    <t>ESP32</t>
   </si>
 </sst>
 </file>
@@ -1379,7 +1382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1474,6 +1477,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1585,7 +1595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1668,6 +1678,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -30137,10 +30151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30591,7 +30605,7 @@
         <v>414</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D24" s="52" t="s">
         <v>416</v>
@@ -30608,7 +30622,7 @@
         <v>415</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>419</v>
@@ -30619,10 +30633,10 @@
         <v>413</v>
       </c>
       <c r="B26" s="47" t="s">
+        <v>427</v>
+      </c>
+      <c r="D26" s="34" t="s">
         <v>428</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>429</v>
       </c>
       <c r="E26" s="33" t="s">
         <v>419</v>
@@ -30633,10 +30647,10 @@
         <v>413</v>
       </c>
       <c r="B27" s="47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E27" s="33" t="s">
         <v>419</v>
@@ -30647,10 +30661,10 @@
         <v>413</v>
       </c>
       <c r="B28" s="47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E28" s="33" t="s">
         <v>419</v>
@@ -30661,10 +30675,10 @@
         <v>413</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E29" s="33" t="s">
         <v>419</v>
@@ -30675,10 +30689,10 @@
         <v>413</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>419</v>
@@ -30689,10 +30703,10 @@
         <v>413</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E31" s="33" t="s">
         <v>419</v>
@@ -30703,7 +30717,7 @@
         <v>413</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C32" s="43" t="s">
         <v>418</v>
@@ -30715,39 +30729,34 @@
         <v>419</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D33" s="43"/>
-    </row>
-    <row r="34" spans="4:4" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="D34" s="52" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D35" s="55" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" s="56" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="56" t="s">
+        <v>440</v>
+      </c>
+      <c r="B33" s="57" t="s">
+        <v>441</v>
+      </c>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57" t="s">
+        <v>442</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D34" s="52"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D35" s="55"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D38" s="43"/>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D39" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D40" t="s">
-        <v>442</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D35" r:id="rId1" xr:uid="{C8692CF0-A15A-4C1F-9AEA-E895533DB497}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -30756,7 +30765,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -31374,13 +31383,13 @@
         <v>413</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C30" s="51" t="s">
         <v>261</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F30" s="33" t="s">
         <v>419</v>

</xml_diff>

<commit_message>
updated the dfplayer library
</commit_message>
<xml_diff>
--- a/SN4 comms values.xlsx
+++ b/SN4 comms values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\SN4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C58C9A-942F-416E-91F1-92639DF3B5B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987D9633-98D4-41C6-A98B-6D03E942DE10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MQTT topics" sheetId="1" state="hidden" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Recieved on Microbit" sheetId="5" r:id="rId3"/>
     <sheet name="Actions" sheetId="2" state="hidden" r:id="rId4"/>
     <sheet name="SN2 Pins" sheetId="3" state="hidden" r:id="rId5"/>
-    <sheet name="S4 Pins" sheetId="8" r:id="rId6"/>
+    <sheet name="SN4 Pins" sheetId="8" r:id="rId6"/>
     <sheet name="BBC Links" sheetId="9" r:id="rId7"/>
     <sheet name="SN3 Pins" sheetId="7" state="hidden" r:id="rId8"/>
     <sheet name="SN1 - Space Rocket" sheetId="4" state="hidden" r:id="rId9"/>
@@ -30142,8 +30142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B35" sqref="A35:B35"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30796,7 +30796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1F20C5-E431-4F51-B98A-61CA1E4D1DB8}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -37370,8 +37370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1006EC9-F903-45E1-9B2E-3BBE97776EFB}">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
moving from UART to i2c
</commit_message>
<xml_diff>
--- a/SN4 comms values.xlsx
+++ b/SN4 comms values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\SN4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987D9633-98D4-41C6-A98B-6D03E942DE10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B72700-AD11-48A0-AE51-8E3A974BA7BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="447">
   <si>
     <t>Action</t>
   </si>
@@ -1036,9 +1036,6 @@
     <t>E15</t>
   </si>
   <si>
-    <t>E16</t>
-  </si>
-  <si>
     <t>Z1</t>
   </si>
   <si>
@@ -1374,6 +1371,18 @@
   <si>
     <t>Returns IP address</t>
   </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>Requests next message from ESP32</t>
+  </si>
 </sst>
 </file>
 
@@ -1393,23 +1402,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1417,22 +1430,26 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1477,9 +1494,10 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1558,6 +1576,12 @@
         <bgColor rgb="FF92CDDC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1588,7 +1612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1671,6 +1695,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -30142,8 +30178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30172,7 +30208,7 @@
         <v>267</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>2</v>
@@ -30183,7 +30219,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C2" s="49" t="s">
         <v>292</v>
@@ -30195,7 +30231,7 @@
         <v>295</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -30203,7 +30239,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="33" t="s">
@@ -30213,7 +30249,7 @@
         <v>295</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -30221,7 +30257,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="33" t="s">
@@ -30231,7 +30267,7 @@
         <v>295</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -30239,7 +30275,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C5" s="49" t="s">
         <v>297</v>
@@ -30251,7 +30287,7 @@
         <v>295</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -30259,7 +30295,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="33" t="s">
@@ -30269,7 +30305,7 @@
         <v>295</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -30277,7 +30313,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="33" t="s">
@@ -30287,7 +30323,7 @@
         <v>295</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -30295,7 +30331,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="33" t="s">
@@ -30305,7 +30341,7 @@
         <v>295</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -30313,17 +30349,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C9" s="49"/>
       <c r="D9" s="33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>295</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -30331,7 +30367,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="33" t="s">
@@ -30341,7 +30377,7 @@
         <v>295</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30349,19 +30385,19 @@
         <v>105</v>
       </c>
       <c r="B11" s="43" t="s">
+        <v>340</v>
+      </c>
+      <c r="C11" s="49" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="D11" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>343</v>
-      </c>
       <c r="E11" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30369,19 +30405,19 @@
         <v>105</v>
       </c>
       <c r="B12" s="43" t="s">
+        <v>343</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>348</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C12" s="51" t="s">
-        <v>349</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>345</v>
-      </c>
       <c r="E12" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F12" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30389,19 +30425,19 @@
         <v>105</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C13" s="51" t="s">
+        <v>349</v>
+      </c>
+      <c r="D13" s="52" t="s">
         <v>350</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>351</v>
-      </c>
       <c r="E13" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30409,19 +30445,19 @@
         <v>166</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C14" s="51" t="s">
+        <v>353</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>356</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>354</v>
       </c>
-      <c r="D14" s="52" t="s">
-        <v>357</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>355</v>
-      </c>
       <c r="F14" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30429,19 +30465,19 @@
         <v>166</v>
       </c>
       <c r="B15" s="43" t="s">
+        <v>352</v>
+      </c>
+      <c r="C15" s="51" t="s">
         <v>353</v>
       </c>
-      <c r="C15" s="51" t="s">
-        <v>354</v>
-      </c>
       <c r="D15" s="52" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30449,19 +30485,19 @@
         <v>271</v>
       </c>
       <c r="B16" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="C16" s="54" t="s">
         <v>360</v>
       </c>
-      <c r="C16" s="54" t="s">
-        <v>361</v>
-      </c>
       <c r="D16" s="34" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>273</v>
       </c>
       <c r="F16" s="54" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30469,121 +30505,121 @@
         <v>271</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>274</v>
       </c>
       <c r="F17" s="54" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="33" t="s">
+        <v>371</v>
+      </c>
+      <c r="B18" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="C18" s="51" t="s">
         <v>373</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="D18" s="52" t="s">
         <v>374</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="E18" s="33" t="s">
         <v>375</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C20" s="51" t="s">
+        <v>434</v>
+      </c>
+      <c r="D20" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="D20" s="52" t="s">
-        <v>436</v>
-      </c>
       <c r="E20" s="33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30591,13 +30627,13 @@
         <v>151</v>
       </c>
       <c r="B24" s="43" t="s">
+        <v>407</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D24" s="52" t="s">
         <v>408</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>409</v>
       </c>
       <c r="E24" s="33" t="s">
         <v>269</v>
@@ -30608,13 +30644,13 @@
         <v>151</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>270</v>
@@ -30622,141 +30658,150 @@
     </row>
     <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="33" t="s">
+        <v>410</v>
+      </c>
+      <c r="B26" s="43" t="s">
         <v>411</v>
       </c>
-      <c r="B26" s="43" t="s">
-        <v>412</v>
-      </c>
       <c r="C26" s="47" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B28" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="D28" s="34" t="s">
         <v>420</v>
       </c>
-      <c r="D28" s="34" t="s">
-        <v>421</v>
-      </c>
       <c r="E28" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C34" s="43" t="s">
+        <v>415</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>414</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>416</v>
       </c>
-      <c r="D34" s="52" t="s">
-        <v>415</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="33"/>
-      <c r="B35" s="47"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="33"/>
+    </row>
+    <row r="35" spans="1:5" s="59" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="56" t="s">
+        <v>445</v>
+      </c>
+      <c r="B35" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="C35" s="57"/>
+      <c r="D35" s="61" t="s">
+        <v>446</v>
+      </c>
+      <c r="E35" s="56" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="33"/>
@@ -30797,7 +30842,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30831,7 +30876,7 @@
         <v>267</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -30852,7 +30897,7 @@
         <v>295</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -30873,7 +30918,7 @@
         <v>295</v>
       </c>
       <c r="G3" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -30894,7 +30939,7 @@
         <v>295</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -30915,7 +30960,7 @@
         <v>294</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -30936,7 +30981,7 @@
         <v>294</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -30947,17 +30992,17 @@
         <v>312</v>
       </c>
       <c r="C7" s="49" t="s">
+        <v>405</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>406</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>407</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="33" t="s">
         <v>269</v>
       </c>
       <c r="G7" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -30968,17 +31013,17 @@
         <v>313</v>
       </c>
       <c r="C8" s="49" t="s">
+        <v>405</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>406</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>407</v>
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="33" t="s">
         <v>270</v>
       </c>
       <c r="G8" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -30999,7 +31044,7 @@
         <v>273</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -31020,7 +31065,7 @@
         <v>274</v>
       </c>
       <c r="G10" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -31037,11 +31082,11 @@
         <v>291</v>
       </c>
       <c r="E11" s="33"/>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="56" t="s">
         <v>276</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -31058,11 +31103,11 @@
         <v>291</v>
       </c>
       <c r="E12" s="33"/>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="56" t="s">
         <v>277</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -31079,11 +31124,11 @@
         <v>291</v>
       </c>
       <c r="E13" s="33"/>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="56" t="s">
         <v>278</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -31100,11 +31145,11 @@
         <v>291</v>
       </c>
       <c r="E14" s="33"/>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="56" t="s">
         <v>279</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -31121,11 +31166,11 @@
         <v>291</v>
       </c>
       <c r="E15" s="33"/>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="56" t="s">
         <v>280</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -31142,11 +31187,11 @@
         <v>291</v>
       </c>
       <c r="E16" s="33"/>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="56" t="s">
         <v>281</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -31163,11 +31208,11 @@
         <v>291</v>
       </c>
       <c r="E17" s="33"/>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="56" t="s">
         <v>282</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -31184,11 +31229,11 @@
         <v>291</v>
       </c>
       <c r="E18" s="33"/>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="56" t="s">
         <v>306</v>
       </c>
       <c r="G18" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -31205,11 +31250,11 @@
         <v>291</v>
       </c>
       <c r="E19" s="33"/>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="56" t="s">
         <v>283</v>
       </c>
       <c r="G19" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -31226,11 +31271,11 @@
         <v>291</v>
       </c>
       <c r="E20" s="33"/>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="56" t="s">
         <v>284</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -31247,11 +31292,11 @@
         <v>291</v>
       </c>
       <c r="E21" s="33"/>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="56" t="s">
         <v>285</v>
       </c>
       <c r="G21" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -31268,11 +31313,11 @@
         <v>291</v>
       </c>
       <c r="E22" s="33"/>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="56" t="s">
         <v>286</v>
       </c>
       <c r="G22" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -31289,11 +31334,11 @@
         <v>291</v>
       </c>
       <c r="E23" s="33"/>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="56" t="s">
         <v>287</v>
       </c>
       <c r="G23" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
@@ -31310,11 +31355,11 @@
         <v>291</v>
       </c>
       <c r="E24" s="33"/>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="56" t="s">
         <v>288</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -31331,100 +31376,100 @@
         <v>291</v>
       </c>
       <c r="E25" s="33"/>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="56" t="s">
         <v>289</v>
       </c>
       <c r="G25" s="43" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="33" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="43" t="s">
-        <v>331</v>
-      </c>
-      <c r="C26" s="47" t="s">
+      <c r="B26" s="57" t="s">
+        <v>443</v>
+      </c>
+      <c r="C26" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33" t="s">
+      <c r="E26" s="56"/>
+      <c r="F26" s="56" t="s">
         <v>290</v>
       </c>
-      <c r="G26" s="43" t="s">
-        <v>366</v>
+      <c r="G26" s="57" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B27" s="43" t="s">
+        <v>383</v>
+      </c>
+      <c r="C27" s="51" t="s">
         <v>384</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="D27" s="33" t="s">
         <v>385</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="F27" s="33" t="s">
         <v>386</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B28" s="43" t="s">
+        <v>387</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="D28" s="33" t="s">
         <v>388</v>
       </c>
-      <c r="C28" s="51" t="s">
-        <v>385</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>389</v>
-      </c>
       <c r="F28" s="33" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>210</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C30" s="51" t="s">
         <v>261</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
@@ -37403,7 +37448,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -37454,7 +37499,7 @@
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>62</v>
@@ -37484,7 +37529,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="53" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B8" s="53" t="s">
         <v>88</v>
@@ -37494,12 +37539,12 @@
         <v>90</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="53" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B9" s="53" t="s">
         <v>96</v>
@@ -37509,12 +37554,12 @@
         <v>97</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="53" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B10" s="53" t="s">
         <v>112</v>
@@ -37524,7 +37569,7 @@
         <v>114</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -37539,12 +37584,12 @@
         <v>126</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="53" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B12" s="53" t="s">
         <v>130</v>
@@ -37554,12 +37599,12 @@
         <v>131</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="53" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B13" s="53" t="s">
         <v>133</v>
@@ -37569,12 +37614,12 @@
         <v>134</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="53" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B14" s="53" t="s">
         <v>137</v>
@@ -37584,7 +37629,7 @@
         <v>138</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41591,22 +41636,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" s="55" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" s="55" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -41655,7 +41700,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -41727,7 +41772,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>88</v>
@@ -41754,7 +41799,7 @@
         <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41766,7 +41811,7 @@
         <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41778,7 +41823,7 @@
         <v>131</v>
       </c>
       <c r="E12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41790,7 +41835,7 @@
         <v>134</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>